<commit_message>
Ecriture de la présentation orale (Fait jusqu'à Langmuir)
</commit_message>
<xml_diff>
--- a/Jets non-défléchi&défléchi.xlsx
+++ b/Jets non-défléchi&défléchi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxiBrioche\Documents\DOSSIER GENERAL\Canada\Université\PHYS EXP 5\S&amp;G\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxiBrioche\PycharmProjects\S-G\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62050F13-DCF5-4BA7-AF00-23AEE937958A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDD3707-AB4A-42B4-B15F-40F4772A5063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{32C9D96F-FB2C-420A-8116-55744F307968}"/>
   </bookViews>
@@ -254,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -277,6 +277,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71BDFFA-B18B-4E15-8C33-A99AF294E99E}">
-  <dimension ref="B1:T22"/>
+  <dimension ref="B1:T32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,7 +1518,26 @@
         <v>2.7134189566127166E-2</v>
       </c>
     </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G28" s="22"/>
+      <c r="M28" s="22"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G29" s="22"/>
+      <c r="M29" s="22"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G30" s="22"/>
+      <c r="M30" s="22"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G31" s="22"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G32" s="22"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>